<commit_message>
updated harvester configuration resistors and removed cap solder link
</commit_message>
<xml_diff>
--- a/resources/energy_harvester/bq25505_70_Design_Help_V1_3.xlsx
+++ b/resources/energy_harvester/bq25505_70_Design_Help_V1_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjeremy\Downloads\Batteryless\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjeremy\Downloads\Tup\xihe\resources\energy_harvester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE1D0CE-60BB-4862-84DC-2E875EC390E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D7B42-AC01-4847-BA39-972417B77083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15135" yWindow="1710" windowWidth="21450" windowHeight="20385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18855" yWindow="2790" windowWidth="23565" windowHeight="19035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bq25505(70" sheetId="1" r:id="rId1"/>
@@ -1843,9 +1843,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>22</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>110490</xdr:colOff>
           <xdr:row>65</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>156210</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2179,9 +2179,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C20" sqref="C20"/>
+      <selection pane="topRight" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2389,7 +2389,7 @@
         <v>8</v>
       </c>
       <c r="I8" s="11">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>1</v>
@@ -2442,7 +2442,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="11">
-        <v>2.5</v>
+        <v>3.3</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>1</v>
@@ -2455,7 +2455,7 @@
         <v>44</v>
       </c>
       <c r="O9" s="11">
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>1</v>
@@ -2582,15 +2582,15 @@
       </c>
       <c r="I13" s="28">
         <f>C1/I9*I7</f>
-        <v>6.2919999999999998</v>
+        <v>4.7666666666666675</v>
       </c>
       <c r="J13" s="46">
         <f>IF(I13&gt;1,VLOOKUP(I13*10,$AA$27:$AA$133,1)/10,IF(I13&gt;0.099,VLOOKUP(I13*100,$AB$27:$AB$133,1)/100,VLOOKUP(I13*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>6.1899999999999995</v>
+        <v>4.75</v>
       </c>
       <c r="K13" s="46">
         <f ca="1">IF(I13&gt;1,OFFSET($AA$27,MATCH(I13*10,$AA$27:$AA$133,1),0)/10,IF(I13&gt;0.099, OFFSET($AB$27,MATCH(I13*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I13*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>6.34</v>
+        <v>4.87</v>
       </c>
       <c r="L13" s="47" t="s">
         <v>59</v>
@@ -2652,15 +2652,15 @@
       </c>
       <c r="I14" s="28">
         <f>(I8/C1-1)*I13</f>
-        <v>5.1480000000000006</v>
+        <v>5.0818181818181838</v>
       </c>
       <c r="J14" s="46">
         <f>IF(I14&gt;1,VLOOKUP(I14*10,$AA$27:$AA$133,1)/10,IF(I14&gt;0.099,VLOOKUP(I14*100,$AB$27:$AB$133,1)/100,VLOOKUP(I14*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>5.1100000000000003</v>
+        <v>4.99</v>
       </c>
       <c r="K14" s="46">
         <f ca="1">IF(I14&gt;1,OFFSET($AA$27,MATCH(I14*10,$AA$27:$AA$133,1),0)/10,IF(I14&gt;0.099, OFFSET($AB$27,MATCH(I14*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I14*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>5.2299999999999995</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="L14" s="47" t="s">
         <v>59</v>
@@ -2670,15 +2670,15 @@
       </c>
       <c r="O14" s="28">
         <f>IF(O8*$C$1/O9&lt;=10, O8*$C$1/O9, O8*$C$1/O9-10)</f>
-        <v>4.7666666666666675</v>
+        <v>6.2919999999999998</v>
       </c>
       <c r="P14" s="46">
         <f>IF(O14&gt;1,VLOOKUP(O14*10,$AA$26:$AA$132,1)/10,IF(O14&gt;0.099,VLOOKUP(O14*100,$AB$26:$AB$132,1)/100,VLOOKUP(O14*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>4.75</v>
+        <v>6.1899999999999995</v>
       </c>
       <c r="Q14" s="46">
         <f ca="1">IF(O14&gt;1,OFFSET($AA$26,MATCH(O14*10,$AA$26:$AA$132,1),0)/10,IF(O14&gt;0.099, OFFSET($AB$26,MATCH(O14*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O14*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>4.87</v>
+        <v>6.34</v>
       </c>
       <c r="R14" s="47" t="s">
         <v>59</v>
@@ -2729,15 +2729,15 @@
       </c>
       <c r="I15" s="28">
         <f>I7-I13-I14</f>
-        <v>1.5599999999999996</v>
+        <v>3.1515151515151487</v>
       </c>
       <c r="J15" s="46">
         <f>IF(I15&gt;1,VLOOKUP(I15*10,$AA$27:$AA$133,1)/10,IF(I15&gt;0.099,VLOOKUP(I15*100,$AB$27:$AB$133,1)/100,VLOOKUP(I15*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>1.54</v>
+        <v>3.09</v>
       </c>
       <c r="K15" s="46">
         <f ca="1">IF(I15&gt;1,OFFSET($AA$27,MATCH(I15*10,$AA$27:$AA$133,1),0)/10,IF(I15&gt;0.099, OFFSET($AB$27,MATCH(I15*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I15*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>1.58</v>
+        <v>3.16</v>
       </c>
       <c r="L15" s="47" t="s">
         <v>59</v>
@@ -2804,11 +2804,11 @@
       <c r="I16" s="16"/>
       <c r="J16" s="46">
         <f>C1*(1+J14/J13)</f>
-        <v>2.2088852988691441</v>
+        <v>2.4811368421052631</v>
       </c>
       <c r="K16" s="46">
         <f ca="1">C1*(1+K14/K13)</f>
-        <v>2.2081545741324922</v>
+        <v>2.4796303901437375</v>
       </c>
       <c r="L16" s="47" t="s">
         <v>1</v>
@@ -2818,15 +2818,15 @@
       </c>
       <c r="O16" s="28">
         <f>IF(O8*$C$1/O9&lt;=10, O8-O14, O8-O14-10)</f>
-        <v>8.2333333333333325</v>
+        <v>6.7080000000000002</v>
       </c>
       <c r="P16" s="46">
         <f>IF(O16&gt;1,VLOOKUP(O16*10,$AA$26:$AA$132,1)/10,IF(O16&gt;0.099,VLOOKUP(O16*100,$AB$26:$AB$132,1)/100,VLOOKUP(O16*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>8.0599999999999987</v>
+        <v>6.65</v>
       </c>
       <c r="Q16" s="46">
         <f ca="1">IF(O16&gt;1,OFFSET($AA$26,MATCH(O16*10,$AA$26:$AA$132,1),0)/10,IF(O16&gt;0.099, OFFSET($AB$26,MATCH(O16*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O16*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>8.25</v>
+        <v>6.81</v>
       </c>
       <c r="R16" s="47" t="s">
         <v>59</v>
@@ -2865,11 +2865,11 @@
       <c r="I17" s="16"/>
       <c r="J17" s="46">
         <f>(C1*((J13+J14+J15)/J13))</f>
-        <v>2.5099192245557354</v>
+        <v>3.2682736842105267</v>
       </c>
       <c r="K17" s="53">
         <f ca="1">(C1*((K13+K14+K15)/K13))</f>
-        <v>2.5097003154574131</v>
+        <v>3.2647638603696096</v>
       </c>
       <c r="L17" s="47" t="s">
         <v>1</v>
@@ -2880,11 +2880,11 @@
       <c r="O17" s="16"/>
       <c r="P17" s="46">
         <f>$C$1*(1+P16/(P14+P15))</f>
-        <v>3.2631789473684205</v>
+        <v>2.5099192245557354</v>
       </c>
       <c r="Q17" s="46">
         <f ca="1">$C$1*(1+Q16/(Q14+Q15))</f>
-        <v>3.2597946611909649</v>
+        <v>2.5097003154574131</v>
       </c>
       <c r="R17" s="81" t="s">
         <v>1</v>
@@ -2936,7 +2936,8 @@
         <v>15</v>
       </c>
       <c r="C19" s="11">
-        <v>4.3</v>
+        <f>4.22*0.99</f>
+        <v>4.1777999999999995</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>58</v>
@@ -2947,7 +2948,7 @@
         <v>17</v>
       </c>
       <c r="I19" s="11">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>58</v>
@@ -2958,7 +2959,7 @@
         <v>45</v>
       </c>
       <c r="O19" s="11">
-        <v>4.7</v>
+        <v>6.49</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>58</v>
@@ -2985,7 +2986,8 @@
         <v>16</v>
       </c>
       <c r="C20" s="11">
-        <v>8.1999999999999993</v>
+        <f>8.2*1.01</f>
+        <v>8.282</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>58</v>
@@ -2996,7 +2998,7 @@
         <v>18</v>
       </c>
       <c r="I20" s="11">
-        <v>4.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>58</v>
@@ -3041,7 +3043,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="11">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>58</v>
@@ -3052,7 +3054,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="11">
-        <v>8.1999999999999993</v>
+        <v>6.49</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>58</v>
@@ -3110,14 +3112,14 @@
       </c>
       <c r="C23" s="56">
         <f>$C$1*(1+C20/C19)*3/2</f>
-        <v>5.2761627906976738</v>
+        <v>5.4130252764612958</v>
       </c>
       <c r="D23" s="75" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="57">
         <f>(C23-C9)/C23*100</f>
-        <v>-4.2424242424242546</v>
+        <v>-1.6067673638421085</v>
       </c>
       <c r="F23" s="74" t="s">
         <v>2</v>
@@ -3127,14 +3129,14 @@
       </c>
       <c r="I23" s="56">
         <f>C1*(1+I20/I19)</f>
-        <v>2.2255357142857144</v>
+        <v>2.5229787234042549</v>
       </c>
       <c r="J23" s="70" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="57">
         <f>(I23-I8)/I23*100</f>
-        <v>1.147396293027358</v>
+        <v>0.91077753415414042</v>
       </c>
       <c r="L23" s="74" t="s">
         <v>2</v>
@@ -3144,11 +3146,11 @@
       </c>
       <c r="O23" s="56">
         <f>$C$1*(1+O21/(O19+O20))</f>
-        <v>3.3210638297872341</v>
+        <v>2.42</v>
       </c>
       <c r="P23" s="57">
         <f>(O23-O9)/O23*100</f>
-        <v>0.63424947145878185</v>
+        <v>-3.3057851239669449</v>
       </c>
       <c r="Q23" s="83" t="s">
         <v>2</v>
@@ -3174,14 +3176,14 @@
       </c>
       <c r="I24" s="68">
         <f>(C1*((I19+I20+I21)/I19))</f>
-        <v>2.4848214285714287</v>
+        <v>3.2953191489361702</v>
       </c>
       <c r="J24" s="85" t="s">
         <v>1</v>
       </c>
       <c r="K24" s="69">
         <f>(I24-I9)/I24*100</f>
-        <v>-0.61085159899388475</v>
+        <v>-0.14204545454545037</v>
       </c>
       <c r="L24" s="73" t="s">
         <v>2</v>

</xml_diff>